<commit_message>
Fixed error on Categories
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -686,7 +686,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1127,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deletion for Devices working
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1127,7 +1127,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,13 +1160,13 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>0</v>
@@ -1177,13 +1177,13 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
@@ -1194,13 +1194,13 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>0</v>
@@ -1211,13 +1211,13 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>0</v>
@@ -1228,13 +1228,13 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>0</v>
@@ -1245,13 +1245,13 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
@@ -1262,13 +1262,13 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
@@ -1279,13 +1279,13 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1296,13 +1296,13 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
@@ -1313,13 +1313,13 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -1330,13 +1330,13 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -1347,13 +1347,13 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -1364,13 +1364,13 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
@@ -1381,13 +1381,13 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1398,10 +1398,10 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
@@ -1415,10 +1415,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
@@ -1432,10 +1432,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
@@ -1449,10 +1449,10 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -1466,10 +1466,10 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -1483,10 +1483,10 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1500,10 +1500,10 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -1517,10 +1517,10 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
@@ -1534,10 +1534,10 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
All deletion complete - testing
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1127,7 +1127,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,16 +1160,16 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,16 +1177,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1194,16 +1194,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,16 +1211,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1228,16 +1228,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,16 +1245,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,16 +1262,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,16 +1279,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,16 +1296,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,16 +1313,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,13 +1330,13 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -1347,13 +1347,13 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -1364,13 +1364,13 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
@@ -1381,13 +1381,13 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,16 +1415,16 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,16 +1432,16 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1449,16 +1449,16 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1466,16 +1466,16 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,16 +1483,16 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,16 +1500,16 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1517,16 +1517,16 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,16 +1534,16 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Returned data table results to false
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1127,7 +1127,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,16 +1160,16 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,16 +1177,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1194,16 +1194,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,16 +1211,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1228,16 +1228,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,16 +1245,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,16 +1262,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,16 +1279,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,16 +1296,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,16 +1313,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,13 +1330,13 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -1347,13 +1347,13 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -1364,13 +1364,13 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
@@ -1381,13 +1381,13 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1398,16 +1398,16 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,16 +1415,16 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,16 +1432,16 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1449,16 +1449,16 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1466,16 +1466,16 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,16 +1483,16 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,16 +1500,16 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1517,16 +1517,16 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,16 +1534,16 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>